<commit_message>
Push - 15.10.2024 - Added logic to logout from BOD whenever login is not requested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\BAH_SOSR_DummyBooking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denitsa.katsarska\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D31C2C4-EECF-4004-98B0-0F55A0A4255F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5A54C3-BECA-47D9-9691-C311DEB816BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -402,6 +402,12 @@
   </si>
   <si>
     <t>Number of retries when a SE is encountered</t>
+  </si>
+  <si>
+    <t>BAH_SOSR_BOD_LogoutUrl</t>
+  </si>
+  <si>
+    <t>URL to logout of BOD</t>
   </si>
 </sst>
 </file>
@@ -786,12 +792,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="65.453125" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -839,7 +845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -851,7 +857,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1866,12 +1872,12 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="119.5703125" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="119.54296875" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1908,7 +1914,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2037,7 +2043,7 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3088,17 +3094,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="4" width="113.28515625" customWidth="1"/>
-    <col min="5" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="46.81640625" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="4" width="113.26953125" customWidth="1"/>
+    <col min="5" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3596,7 +3602,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" t="s">
+        <v>127</v>
+      </c>
+    </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Push - 21.11 - Removed all folder paths from Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denitsa.katsarska\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVELOPER\Documents\UiPath\RPA_BAH_SOSR_DummyBooking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5A54C3-BECA-47D9-9691-C311DEB816BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC64C6B-F007-45E8-A6B6-DCCA6B86FEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>BAH_SOSR_ConfirmationErrorMessage</t>
-  </si>
-  <si>
-    <t>UatRPA/BAW/BA Holidays/BA Holidays</t>
   </si>
   <si>
     <t>BAH_SOSR_LoginText</t>
@@ -789,15 +786,15 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="65.453125" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -845,24 +842,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>21</v>
@@ -1872,12 +1867,12 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="119.54296875" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="119.5703125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1914,7 +1909,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1925,7 +1920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2043,7 +2038,7 @@
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2056,68 +2051,68 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="5">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="5">
         <v>3000</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
         <v>107</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
         <v>109</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>110</v>
-      </c>
-      <c r="C21" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
         <v>117</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>118</v>
-      </c>
-      <c r="C22" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
         <v>120</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3094,17 +3089,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="46.81640625" customWidth="1"/>
-    <col min="2" max="2" width="44.453125" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="4" width="113.26953125" customWidth="1"/>
-    <col min="5" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="113.28515625" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3150,9 +3145,6 @@
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
       <c r="D2" t="s">
         <v>42</v>
       </c>
@@ -3164,9 +3156,6 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
-        <v>76</v>
-      </c>
       <c r="D3" t="s">
         <v>44</v>
       </c>
@@ -3178,9 +3167,6 @@
       <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
       <c r="D4" t="s">
         <v>46</v>
       </c>
@@ -3192,9 +3178,6 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
       <c r="D5" t="s">
         <v>48</v>
       </c>
@@ -3206,9 +3189,6 @@
       <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
-        <v>76</v>
-      </c>
       <c r="D6" t="s">
         <v>50</v>
       </c>
@@ -3220,9 +3200,6 @@
       <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
       <c r="D7" t="s">
         <v>52</v>
       </c>
@@ -3234,9 +3211,6 @@
       <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
       <c r="D8" t="s">
         <v>54</v>
       </c>
@@ -3248,9 +3222,6 @@
       <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
       <c r="D9" t="s">
         <v>56</v>
       </c>
@@ -3262,9 +3233,6 @@
       <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
       <c r="D10" t="s">
         <v>59</v>
       </c>
@@ -3276,9 +3244,6 @@
       <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
-        <v>76</v>
-      </c>
       <c r="D11" t="s">
         <v>61</v>
       </c>
@@ -3290,9 +3255,6 @@
       <c r="B12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
       <c r="D12" t="s">
         <v>63</v>
       </c>
@@ -3304,9 +3266,6 @@
       <c r="B13" t="s">
         <v>65</v>
       </c>
-      <c r="C13" t="s">
-        <v>76</v>
-      </c>
       <c r="D13" t="s">
         <v>66</v>
       </c>
@@ -3318,9 +3277,6 @@
       <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" t="s">
-        <v>76</v>
-      </c>
       <c r="D14" t="s">
         <v>68</v>
       </c>
@@ -3332,9 +3288,6 @@
       <c r="B15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
-        <v>76</v>
-      </c>
       <c r="D15" t="s">
         <v>69</v>
       </c>
@@ -3346,9 +3299,6 @@
       <c r="B16" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
-        <v>76</v>
-      </c>
       <c r="D16" t="s">
         <v>73</v>
       </c>
@@ -3360,260 +3310,203 @@
       <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="C17" t="s">
-        <v>76</v>
-      </c>
       <c r="D17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
         <v>77</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
         <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s">
         <v>81</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
         <v>91</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
         <v>93</v>
-      </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
         <v>97</v>
-      </c>
-      <c r="B25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" t="s">
         <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
         <v>100</v>
-      </c>
-      <c r="B28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
         <v>103</v>
-      </c>
-      <c r="B29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
         <v>112</v>
-      </c>
-      <c r="B30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" t="s">
         <v>115</v>
-      </c>
-      <c r="B32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
         <v>122</v>
-      </c>
-      <c r="B33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
         <v>124</v>
-      </c>
-      <c r="B34" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" t="s">
         <v>126</v>
-      </c>
-      <c r="B35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1"/>

</xml_diff>